<commit_message>
Added the database connection
</commit_message>
<xml_diff>
--- a/Guru99ApplicationTest/TestData/TestData.xlsx
+++ b/Guru99ApplicationTest/TestData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saurabh Dhingra\source\repos\Modular Framework 02052020\Guru99ApplicationTest\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CEA0EAC-56C5-4FDE-B711-3BC398E0C99D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FFE739-E154-4EF6-9B65-7234F35279A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -369,7 +369,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>